<commit_message>
Corrected Org Name for GIT ACTIONS
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/RSTK-9230_Cost Transaction Query.xlsx
+++ b/templates/AutomationOrg/RSTK-9230_Cost Transaction Query.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\PKTEst\TestProje\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A09838A-B8CA-4C36-8099-5707F50D5BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C52F6D-DFF8-4923-A81D-1FEA33294FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DB51E305-5BC0-4BB2-AE6B-CC4DBF74AF6A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB51E305-5BC0-4BB2-AE6B-CC4DBF74AF6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Transaction Query" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t xml:space="preserve">Inventory Item Master	</t>
   </si>
@@ -62,7 +62,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="mm\/dd\/yyyy"/>
+    <numFmt numFmtId="164" formatCode="mm\/dd\/yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -115,7 +115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D245C7FE-FD08-42D7-B5E2-E564985D2B08}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,16 +499,6 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="6">
-        <v>44263</v>
-      </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>